<commit_message>
Revisión 2 MA_09_02_CO y Escaleta_MA_09_02_CO
Revisión 2 de guion y escaleta actualizada
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion02/Escaleta_MA_09_02_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion02/Escaleta_MA_09_02_CO.xlsx
@@ -829,9 +829,6 @@
     <t>Refuerza tu aprendizaje: El proceso de racionalización</t>
   </si>
   <si>
-    <t>Proyecto: números grandes y números pequeños</t>
-  </si>
-  <si>
     <t xml:space="preserve">Actividades que propone ejercicios de aplicación de las leyes de la potenciación </t>
   </si>
   <si>
@@ -931,10 +928,13 @@
     <t>Actividad para evaluar el tema La potenciación y la radicación de números reales</t>
   </si>
   <si>
-    <t>Proyecto sobre contextos de medida</t>
-  </si>
-  <si>
     <t>Actividades sobre el tema La potenciación y la radicación de números reales</t>
+  </si>
+  <si>
+    <t>Competencias: números grandes y números pequeños</t>
+  </si>
+  <si>
+    <t>Actividad que propone expresar medidas en notación científica</t>
   </si>
 </sst>
 </file>
@@ -1485,25 +1485,19 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1522,6 +1516,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1941,8 +1941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G16" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="G18" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1974,98 +1974,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="30" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="74" t="s">
+      <c r="C1" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="70" t="s">
+      <c r="D1" s="67" t="s">
         <v>223</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="66" t="s">
         <v>224</v>
       </c>
-      <c r="F1" s="75" t="s">
+      <c r="F1" s="73" t="s">
         <v>225</v>
       </c>
-      <c r="G1" s="65" t="s">
+      <c r="G1" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="68" t="s">
+      <c r="H1" s="64" t="s">
         <v>218</v>
       </c>
-      <c r="I1" s="68" t="s">
+      <c r="I1" s="64" t="s">
         <v>102</v>
       </c>
-      <c r="J1" s="72" t="s">
+      <c r="J1" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="71" t="s">
+      <c r="K1" s="69" t="s">
         <v>219</v>
       </c>
-      <c r="L1" s="65" t="s">
+      <c r="L1" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="73" t="s">
+      <c r="M1" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="73"/>
-      <c r="O1" s="64" t="s">
+      <c r="N1" s="71"/>
+      <c r="O1" s="65" t="s">
         <v>103</v>
       </c>
-      <c r="P1" s="64" t="s">
+      <c r="P1" s="65" t="s">
         <v>226</v>
       </c>
-      <c r="Q1" s="66" t="s">
+      <c r="Q1" s="75" t="s">
         <v>89</v>
       </c>
-      <c r="R1" s="67" t="s">
+      <c r="R1" s="76" t="s">
         <v>90</v>
       </c>
-      <c r="S1" s="66" t="s">
+      <c r="S1" s="75" t="s">
         <v>91</v>
       </c>
-      <c r="T1" s="67" t="s">
+      <c r="T1" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="U1" s="66" t="s">
+      <c r="U1" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="AA1" s="65" t="s">
+      <c r="AA1" s="68" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:27" s="30" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="A2" s="70"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="65"/>
+      <c r="A2" s="67"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="68"/>
       <c r="M2" s="32" t="s">
         <v>94</v>
       </c>
       <c r="N2" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="67"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="67"/>
-      <c r="U2" s="66"/>
-      <c r="AA2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="76"/>
+      <c r="S2" s="75"/>
+      <c r="T2" s="76"/>
+      <c r="U2" s="75"/>
+      <c r="AA2" s="68"/>
     </row>
     <row r="3" spans="1:27" s="34" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
@@ -2094,7 +2094,7 @@
         <v>164</v>
       </c>
       <c r="J3" s="40" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K3" s="41" t="s">
         <v>164</v>
@@ -2224,7 +2224,7 @@
         <v>198</v>
       </c>
       <c r="J5" s="40" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K5" s="41" t="s">
         <v>75</v>
@@ -2293,7 +2293,7 @@
         <v>198</v>
       </c>
       <c r="J6" s="40" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K6" s="41" t="s">
         <v>75</v>
@@ -2360,7 +2360,7 @@
         <v>198</v>
       </c>
       <c r="J7" s="40" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K7" s="41" t="s">
         <v>166</v>
@@ -2421,7 +2421,7 @@
         <v>164</v>
       </c>
       <c r="J8" s="40" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K8" s="41" t="s">
         <v>166</v>
@@ -2484,7 +2484,7 @@
         <v>198</v>
       </c>
       <c r="J9" s="40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K9" s="41" t="s">
         <v>16</v>
@@ -2547,7 +2547,7 @@
         <v>198</v>
       </c>
       <c r="J10" s="40" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K10" s="41" t="s">
         <v>166</v>
@@ -2677,7 +2677,7 @@
         <v>198</v>
       </c>
       <c r="J12" s="40" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K12" s="41" t="s">
         <v>76</v>
@@ -2733,7 +2733,7 @@
       </c>
       <c r="F13" s="42"/>
       <c r="G13" s="39" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H13" s="33">
         <v>11</v>
@@ -2742,7 +2742,7 @@
         <v>198</v>
       </c>
       <c r="J13" s="40" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K13" s="41" t="s">
         <v>75</v>
@@ -2805,7 +2805,7 @@
         <v>23</v>
       </c>
       <c r="J14" s="40" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K14" s="41" t="s">
         <v>75</v>
@@ -2939,7 +2939,7 @@
         <v>23</v>
       </c>
       <c r="J16" s="40" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K16" s="41" t="s">
         <v>75</v>
@@ -3006,7 +3006,7 @@
         <v>198</v>
       </c>
       <c r="J17" s="40" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K17" s="41" t="s">
         <v>75</v>
@@ -3073,7 +3073,7 @@
         <v>198</v>
       </c>
       <c r="J18" s="40" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K18" s="41" t="s">
         <v>75</v>
@@ -3140,7 +3140,7 @@
         <v>164</v>
       </c>
       <c r="J19" s="40" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K19" s="41" t="s">
         <v>75</v>
@@ -3205,7 +3205,7 @@
         <v>164</v>
       </c>
       <c r="J20" s="40" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K20" s="41" t="s">
         <v>76</v>
@@ -3268,7 +3268,7 @@
         <v>198</v>
       </c>
       <c r="J21" s="40" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K21" s="41" t="s">
         <v>76</v>
@@ -3329,7 +3329,7 @@
         <v>198</v>
       </c>
       <c r="J22" s="40" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K22" s="41" t="s">
         <v>76</v>
@@ -3390,7 +3390,7 @@
         <v>198</v>
       </c>
       <c r="J23" s="40" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K23" s="41" t="s">
         <v>76</v>
@@ -3455,7 +3455,7 @@
         <v>198</v>
       </c>
       <c r="J24" s="40" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K24" s="41" t="s">
         <v>76</v>
@@ -3520,7 +3520,7 @@
         <v>198</v>
       </c>
       <c r="J25" s="40" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K25" s="41" t="s">
         <v>75</v>
@@ -3587,7 +3587,7 @@
         <v>164</v>
       </c>
       <c r="J26" s="40" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K26" s="41" t="s">
         <v>76</v>
@@ -3654,7 +3654,7 @@
         <v>198</v>
       </c>
       <c r="J27" s="40" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K27" s="41" t="s">
         <v>76</v>
@@ -3721,7 +3721,7 @@
         <v>198</v>
       </c>
       <c r="J28" s="40" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K28" s="41" t="s">
         <v>76</v>
@@ -3788,7 +3788,7 @@
         <v>198</v>
       </c>
       <c r="J29" s="40" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K29" s="41" t="s">
         <v>75</v>
@@ -3851,7 +3851,7 @@
         <v>198</v>
       </c>
       <c r="J30" s="40" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K30" s="41" t="s">
         <v>76</v>
@@ -3903,7 +3903,7 @@
       </c>
       <c r="F31" s="42"/>
       <c r="G31" s="39" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H31" s="33">
         <v>29</v>
@@ -3912,7 +3912,7 @@
         <v>198</v>
       </c>
       <c r="J31" s="40" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K31" s="41" t="s">
         <v>75</v>
@@ -3975,7 +3975,7 @@
         <v>164</v>
       </c>
       <c r="J32" s="40" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K32" s="41" t="s">
         <v>75</v>
@@ -4036,7 +4036,7 @@
         <v>198</v>
       </c>
       <c r="J33" s="40" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K33" s="41" t="s">
         <v>76</v>
@@ -4097,7 +4097,7 @@
         <v>198</v>
       </c>
       <c r="J34" s="40" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K34" s="41" t="s">
         <v>75</v>
@@ -4151,7 +4151,7 @@
       </c>
       <c r="F35" s="42"/>
       <c r="G35" s="39" t="s">
-        <v>241</v>
+        <v>275</v>
       </c>
       <c r="H35" s="33">
         <v>33</v>
@@ -4160,7 +4160,7 @@
         <v>164</v>
       </c>
       <c r="J35" s="40" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="K35" s="41" t="s">
         <v>75</v>
@@ -4227,7 +4227,7 @@
         <v>198</v>
       </c>
       <c r="J36" s="40" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K36" s="41"/>
       <c r="L36" s="39"/>
@@ -4276,7 +4276,7 @@
         <v>198</v>
       </c>
       <c r="J37" s="40" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K37" s="41" t="s">
         <v>75</v>
@@ -4332,7 +4332,7 @@
       <c r="E38" s="50"/>
       <c r="F38" s="42"/>
       <c r="G38" s="39" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H38" s="33">
         <v>36</v>
@@ -4341,7 +4341,7 @@
         <v>198</v>
       </c>
       <c r="J38" s="63" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K38" s="41"/>
       <c r="L38" s="39"/>
@@ -4453,6 +4453,13 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4467,13 +4474,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K6 K11:K38">

</xml_diff>